<commit_message>
release version final not edit more
</commit_message>
<xml_diff>
--- a/version.final/time_attendance/517100-2567-1-Computer Programing 1.xlsx
+++ b/version.final/time_attendance/517100-2567-1-Computer Programing 1.xlsx
@@ -633,7 +633,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>06:22:24</t>
+          <t>06:42:21</t>
         </is>
       </c>
     </row>
@@ -733,7 +733,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>05:13:31</t>
+          <t>06:38:57</t>
         </is>
       </c>
     </row>

</xml_diff>